<commit_message>
foxed up excel file
</commit_message>
<xml_diff>
--- a/DM Solution Documentaion/Redwood Solution Workbook.xlsx
+++ b/DM Solution Documentaion/Redwood Solution Workbook.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\source\repos\RedwoodRealty\DM Solution Documentaion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Documents/DU/Info4240/RedwoodRealty/DM Solution Documentaion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D836F622-E568-446A-997B-F1C537416D72}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B461C7-FC36-A94E-9F15-127BA888AC60}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="32625" windowHeight="18195" tabRatio="950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="18200" tabRatio="950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
     <sheet name="Data Warehouse" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Locator">'Data Warehouse'!$LCB$524288</definedName>
+    <definedName name="Locator">'Data Warehouse'!$LCB$524286</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="120">
   <si>
     <t>Object Name</t>
   </si>
@@ -80,9 +80,6 @@
     <t>money</t>
   </si>
   <si>
-    <t>nvarchar(50)</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>DWRedwoodBids.dbo.DimDates.Date</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimDates.DateName</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.DimDates.Month</t>
   </si>
   <si>
@@ -134,18 +128,12 @@
     <t>DWRedwoodBids.dbo.DimDates.Year</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimDates.YearName</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList</t>
   </si>
   <si>
     <t>DWRedwoodBids.dbo.FactBids</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.BidDateKey</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList.BidPrice</t>
   </si>
   <si>
@@ -188,12 +176,6 @@
     <t>nvarchar(25)</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.BidAgentKey</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimProperty.PropertyKey</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.DimProperty</t>
   </si>
   <si>
@@ -284,9 +266,6 @@
     <t>DWRedwoodBids.dbo.DimCustomer</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimCustomer.CustomerKey</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Customer.CustomerID</t>
   </si>
   <si>
@@ -314,12 +293,6 @@
     <t>Redwood.dbo.CustAgentList.CustomerID</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.PropertyKey</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.CustomerKey</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.DimProperty.LotSize</t>
   </si>
   <si>
@@ -332,12 +305,6 @@
     <t>Redwood.dbo.Customer</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgentKey</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.ListingDateKey</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Listing.BeginListDate</t>
   </si>
   <si>
@@ -386,13 +353,37 @@
     <t>DWRedwoodBids.dbo.FactBids.DaysOnMarket</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgentID</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimProperty.PropertyID</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimCustomer.CustomerID</t>
+    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgent_AK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgent_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimProperty.Property_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimProperty.Property_AK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimCustomer.Customer_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimCustomer.Customer_AK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.BidDate_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.BidAgent_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.Property_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.ListingDate_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.Customer_SK</t>
   </si>
 </sst>
 </file>
@@ -858,7 +849,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
   </cols>
@@ -873,18 +864,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -901,19 +892,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -935,13 +926,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -952,13 +943,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -969,13 +960,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
@@ -986,13 +977,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>10</v>
@@ -1003,13 +994,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>10</v>
@@ -1020,13 +1011,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>10</v>
@@ -1037,13 +1028,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
@@ -1054,13 +1045,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
@@ -1071,13 +1062,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -1086,32 +1077,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.45" customHeight="1">
+    <row r="11" spans="1:5" ht="14.5" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.45" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.5" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>10</v>
@@ -1122,13 +1113,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
@@ -1139,16 +1130,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>10</v>
@@ -1156,13 +1147,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>10</v>
@@ -1173,115 +1164,115 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>7</v>
@@ -1292,16 +1283,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>10</v>
@@ -1309,13 +1300,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>10</v>
@@ -1326,47 +1317,47 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>10</v>
@@ -1377,13 +1368,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>10</v>
@@ -1394,13 +1385,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>10</v>
@@ -1411,13 +1402,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>10</v>
@@ -1428,98 +1419,98 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>7</v>
@@ -1530,16 +1521,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="5" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>10</v>
@@ -1547,13 +1538,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>10</v>
@@ -1564,84 +1555,84 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>7</v>
@@ -1649,16 +1640,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>10</v>
@@ -1666,16 +1657,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>12</v>
@@ -1683,19 +1674,19 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>20</v>
+      <c r="C46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1705,11 +1696,11 @@
       <c r="B47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>20</v>
+      <c r="C47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>10</v>
@@ -1723,27 +1714,27 @@
         <v>16</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
+      <c r="C49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>10</v>
@@ -1751,69 +1742,35 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="s">
+      <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added YearName & DateName fields to Date table and removed "SK" from date fields on fact table. Updated Documentation accordingly.
</commit_message>
<xml_diff>
--- a/DM Solution Documentaion/Redwood Solution Workbook.xlsx
+++ b/DM Solution Documentaion/Redwood Solution Workbook.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brian/Documents/DU/Info4240/RedwoodRealty/DM Solution Documentaion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Source\Repos\RedwoodRealty\DM Solution Documentaion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B461C7-FC36-A94E-9F15-127BA888AC60}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA1A6DF-ECE3-46C4-A378-F09DE736E542}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="18200" tabRatio="950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="32625" windowHeight="18195" tabRatio="950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
     <sheet name="Data Warehouse" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Locator">'Data Warehouse'!$LCB$524286</definedName>
+    <definedName name="Locator">'Data Warehouse'!$LCB$524288</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
   <si>
     <t>Object Name</t>
   </si>
@@ -371,19 +371,25 @@
     <t>DWRedwoodBids.dbo.DimCustomer.Customer_AK</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.BidDate_SK</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.BidAgent_SK</t>
   </si>
   <si>
     <t>DWRedwoodBids.dbo.Property_SK</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.ListingDate_SK</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.Customer_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.BidDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.ListingDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDates.YearName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDates.DateName</t>
   </si>
 </sst>
 </file>
@@ -849,7 +855,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
   </cols>
@@ -892,19 +898,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -960,7 +966,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -977,7 +983,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
@@ -994,7 +1000,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -1011,7 +1017,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
@@ -1028,7 +1034,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
@@ -1077,7 +1083,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.5" customHeight="1">
+    <row r="11" spans="1:5" ht="14.45" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>107</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.5" customHeight="1">
+    <row r="12" spans="1:5" ht="14.45" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>108</v>
       </c>
@@ -1673,25 +1679,25 @@
       </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="5" t="s">
-        <v>33</v>
+      <c r="A46" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>16</v>
@@ -1707,16 +1713,16 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="5" t="s">
-        <v>32</v>
+      <c r="A48" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="6" t="s">
@@ -1725,15 +1731,15 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="C49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="6" t="s">
@@ -1742,7 +1748,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>16</v>
@@ -1758,19 +1764,53 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added select data for ETL
</commit_message>
<xml_diff>
--- a/DM Solution Documentaion/Redwood Solution Workbook.xlsx
+++ b/DM Solution Documentaion/Redwood Solution Workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Source\Repos\RedwoodRealty\DM Solution Documentaion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\source\repos\RedwoodRealty\DM Solution Documentaion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA1A6DF-ECE3-46C4-A378-F09DE736E542}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB4450B-37B3-4F09-8991-B459C0F18DF6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="32625" windowHeight="18195" tabRatio="950" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Data Warehouse" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Locator">'Data Warehouse'!$LCB$524288</definedName>
+    <definedName name="Locator">'Data Warehouse'!$LCB$524289</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="124">
   <si>
     <t>Object Name</t>
   </si>
@@ -104,30 +104,6 @@
     <t>DWRedwoodBids</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimDates</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.DateKey</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.Date</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.Month</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.MonthName</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.Quarter</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.QuarterName</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.Year</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList</t>
   </si>
   <si>
@@ -242,27 +218,6 @@
     <t>Redwood.dbo.Agent</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.FirstName</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.LastName</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.Title</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.HireDate</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.LicenseDate</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.LicenseStatus</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.DimCustomer</t>
   </si>
   <si>
@@ -353,12 +308,6 @@
     <t>DWRedwoodBids.dbo.FactBids.DaysOnMarket</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgent_AK</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimBidAgent.BidAgent_SK</t>
-  </si>
-  <si>
     <t>DWRedwoodBids.dbo.DimProperty.Property_SK</t>
   </si>
   <si>
@@ -386,17 +335,74 @@
     <t>DWRedwoodBids.dbo.ListingDate</t>
   </si>
   <si>
-    <t>DWRedwoodBids.dbo.DimDates.YearName</t>
-  </si>
-  <si>
-    <t>DWRedwoodBids.dbo.DimDates.DateName</t>
+    <t>DWRedwoodBids.dbo.DimDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.DateKey</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.Date</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.DateName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.Year</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.YearName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.Quarter</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.QuarterName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.Month</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimDate.MonthName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.ListingAgent_SK</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.ListingAgentID</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.BidAgent_SK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.BidAgent_AK</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.FirstName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.LastName</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.Title</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.HireDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.LicenseDate</t>
+  </si>
+  <si>
+    <t>DWRedwoodBids.dbo.DimAgent.LicenseStatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +437,11 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica 65 Medium"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica 65 Medium"/>
@@ -491,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -500,6 +511,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,12 +867,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -868,7 +880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -876,7 +888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -898,22 +910,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -947,15 +959,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -964,15 +976,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
-        <v>118</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
@@ -981,15 +993,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>115</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>10</v>
@@ -998,15 +1010,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>116</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>10</v>
@@ -1015,15 +1027,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>117</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>10</v>
@@ -1032,49 +1044,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>119</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
-        <v>106</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>17</v>
@@ -1083,508 +1095,508 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>107</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>108</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>104</v>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="5" t="s">
+      <c r="B36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>102</v>
+        <v>11</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>84</v>
+      <c r="C40" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>41</v>
@@ -1593,77 +1605,77 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="C44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>16</v>
@@ -1675,80 +1687,80 @@
         <v>19</v>
       </c>
       <c r="E45" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="5" t="s">
-        <v>33</v>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="C47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="6" t="s">
-        <v>120</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="C48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="C49" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>16</v>
@@ -1760,57 +1772,74 @@
         <v>19</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="C51" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="C52" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>